<commit_message>
Cleaning jupyter notebook for publishing
</commit_message>
<xml_diff>
--- a/Data_S1.xlsx
+++ b/Data_S1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tfuqua\Dropbox\Wagner_group\Writing\Promoter_Islands_Manuscript\PI_manuscript_v01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tfuqua\Documents\GitHub\promoter_islands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727C16CF-A86E-4D12-9D0A-FAF1C8374197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39DF506-AC9D-40D8-99F3-B82525037146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="17400" activeTab="1" xr2:uid="{9179D6F8-F47B-49AE-A737-A3E6992016B5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{9179D6F8-F47B-49AE-A737-A3E6992016B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Primers" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="237">
   <si>
     <t>Category</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Primer to amplify inserts and clone them into pMR1, flanked with EcoR (GAATTC) and BamHI (GGATCC) cut sites</t>
   </si>
   <si>
-    <t>CAACCTCCCTTGCGA</t>
-  </si>
-  <si>
     <t>pMR1_construct_gibson_assembly_reverse</t>
   </si>
   <si>
@@ -120,156 +117,6 @@
     <t>CAATGCTAGCGGATCCTTGCG</t>
   </si>
   <si>
-    <t>PI75_fwd</t>
-  </si>
-  <si>
-    <t>PI75_rev</t>
-  </si>
-  <si>
-    <t>PI18_fwd</t>
-  </si>
-  <si>
-    <t>PI18_rev</t>
-  </si>
-  <si>
-    <t>PI19_fwd</t>
-  </si>
-  <si>
-    <t>PI19_rev</t>
-  </si>
-  <si>
-    <t>PI3_fwd</t>
-  </si>
-  <si>
-    <t>PI3_rev</t>
-  </si>
-  <si>
-    <t>PI52_fwd</t>
-  </si>
-  <si>
-    <t>PI52_rev</t>
-  </si>
-  <si>
-    <t>PI72_fwd</t>
-  </si>
-  <si>
-    <t>PI72_rev</t>
-  </si>
-  <si>
-    <t>PI25_fwd</t>
-  </si>
-  <si>
-    <t>PI25_rev</t>
-  </si>
-  <si>
-    <t>PI55_fwd</t>
-  </si>
-  <si>
-    <t>PI55_rev</t>
-  </si>
-  <si>
-    <t>PI1_fwd</t>
-  </si>
-  <si>
-    <t>PI1_rev</t>
-  </si>
-  <si>
-    <t>PI45_fwd</t>
-  </si>
-  <si>
-    <t>PI45_rev</t>
-  </si>
-  <si>
-    <t>PI64_fwd</t>
-  </si>
-  <si>
-    <t>PI64_rev</t>
-  </si>
-  <si>
-    <t>PI6_fwd</t>
-  </si>
-  <si>
-    <t>PI6_rev</t>
-  </si>
-  <si>
-    <t>PI29_fwd</t>
-  </si>
-  <si>
-    <t>PI29_rev</t>
-  </si>
-  <si>
-    <t>PI24_fwd</t>
-  </si>
-  <si>
-    <t>PI24_rev</t>
-  </si>
-  <si>
-    <t>PI20_fwd</t>
-  </si>
-  <si>
-    <t>PI20_rev</t>
-  </si>
-  <si>
-    <t>PI4_fwd</t>
-  </si>
-  <si>
-    <t>PI4_rev</t>
-  </si>
-  <si>
-    <t>PI76_fwd</t>
-  </si>
-  <si>
-    <t>PI76_rev</t>
-  </si>
-  <si>
-    <t>PI11_fwd</t>
-  </si>
-  <si>
-    <t>PI11_rev</t>
-  </si>
-  <si>
-    <t>PI59_fwd</t>
-  </si>
-  <si>
-    <t>PI59_rev</t>
-  </si>
-  <si>
-    <t>PI26_fwd</t>
-  </si>
-  <si>
-    <t>PI26_rev</t>
-  </si>
-  <si>
-    <t>PI58_fwd</t>
-  </si>
-  <si>
-    <t>PI58_rev</t>
-  </si>
-  <si>
-    <t>PI30_fwd</t>
-  </si>
-  <si>
-    <t>PI30_rev</t>
-  </si>
-  <si>
-    <t>PI73_fwd</t>
-  </si>
-  <si>
-    <t>PI73_rev</t>
-  </si>
-  <si>
-    <t>PI38_fwd</t>
-  </si>
-  <si>
-    <t>PI38_rev</t>
-  </si>
-  <si>
-    <t>PI78_fwd</t>
-  </si>
-  <si>
-    <t>PI78_rev</t>
-  </si>
-  <si>
     <t>Promoter Island (PI) sequence</t>
   </si>
   <si>
@@ -670,13 +517,244 @@
   </si>
   <si>
     <t>attactaattggaatttgatgttgctatattgaggtctatattaataatgcctgtgaatggtatttttgatgtatttgatatgttatcaatttatattatttacaaactaattgtttcaaataatacatggctgattatgcggaaataaa</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>P6</t>
+  </si>
+  <si>
+    <t>P7</t>
+  </si>
+  <si>
+    <t>P8</t>
+  </si>
+  <si>
+    <t>P9</t>
+  </si>
+  <si>
+    <t>P10</t>
+  </si>
+  <si>
+    <t>P11</t>
+  </si>
+  <si>
+    <t>P12</t>
+  </si>
+  <si>
+    <t>P13</t>
+  </si>
+  <si>
+    <t>P14</t>
+  </si>
+  <si>
+    <t>P15</t>
+  </si>
+  <si>
+    <t>P16</t>
+  </si>
+  <si>
+    <t>P17</t>
+  </si>
+  <si>
+    <t>P18</t>
+  </si>
+  <si>
+    <t>P19</t>
+  </si>
+  <si>
+    <t>P20</t>
+  </si>
+  <si>
+    <t>P21</t>
+  </si>
+  <si>
+    <t>P22</t>
+  </si>
+  <si>
+    <t>P23</t>
+  </si>
+  <si>
+    <t>P24</t>
+  </si>
+  <si>
+    <t>P25</t>
+  </si>
+  <si>
+    <t>CAACCTCCCTTGCGAATTTTAATTAAGGCTGAATTC</t>
+  </si>
+  <si>
+    <t>ATTCTAGGTACCCGGGGATCGCGATCGCAAGGATCC</t>
+  </si>
+  <si>
+    <t>P1_fwd</t>
+  </si>
+  <si>
+    <t>P1_rev</t>
+  </si>
+  <si>
+    <t>P2_fwd</t>
+  </si>
+  <si>
+    <t>P2_rev</t>
+  </si>
+  <si>
+    <t>P3_fwd</t>
+  </si>
+  <si>
+    <t>P3_rev</t>
+  </si>
+  <si>
+    <t>P4_fwd</t>
+  </si>
+  <si>
+    <t>P4_rev</t>
+  </si>
+  <si>
+    <t>P5_fwd</t>
+  </si>
+  <si>
+    <t>P5_rev</t>
+  </si>
+  <si>
+    <t>P6_fwd</t>
+  </si>
+  <si>
+    <t>P6_rev</t>
+  </si>
+  <si>
+    <t>P7_fwd</t>
+  </si>
+  <si>
+    <t>P7_rev</t>
+  </si>
+  <si>
+    <t>P8_fwd</t>
+  </si>
+  <si>
+    <t>P8_rev</t>
+  </si>
+  <si>
+    <t>P9_fwd</t>
+  </si>
+  <si>
+    <t>P9_rev</t>
+  </si>
+  <si>
+    <t>P10_fwd</t>
+  </si>
+  <si>
+    <t>P10_rev</t>
+  </si>
+  <si>
+    <t>P11_fwd</t>
+  </si>
+  <si>
+    <t>P11_rev</t>
+  </si>
+  <si>
+    <t>P12_fwd</t>
+  </si>
+  <si>
+    <t>P12_rev</t>
+  </si>
+  <si>
+    <t>P13_fwd</t>
+  </si>
+  <si>
+    <t>P13_rev</t>
+  </si>
+  <si>
+    <t>P14_fwd</t>
+  </si>
+  <si>
+    <t>P14_rev</t>
+  </si>
+  <si>
+    <t>P15_fwd</t>
+  </si>
+  <si>
+    <t>P15_rev</t>
+  </si>
+  <si>
+    <t>P16_fwd</t>
+  </si>
+  <si>
+    <t>P16_rev</t>
+  </si>
+  <si>
+    <t>P17_fwd</t>
+  </si>
+  <si>
+    <t>P18_rev</t>
+  </si>
+  <si>
+    <t>P17_rev</t>
+  </si>
+  <si>
+    <t>P18_fwd</t>
+  </si>
+  <si>
+    <t>P19_fwd</t>
+  </si>
+  <si>
+    <t>P19_rev</t>
+  </si>
+  <si>
+    <t>P20_fwd</t>
+  </si>
+  <si>
+    <t>P20_rev</t>
+  </si>
+  <si>
+    <t>P21_fwd</t>
+  </si>
+  <si>
+    <t>P21_rev</t>
+  </si>
+  <si>
+    <t>P22_fwd</t>
+  </si>
+  <si>
+    <t>P22_rev</t>
+  </si>
+  <si>
+    <t>P23_fwd</t>
+  </si>
+  <si>
+    <t>P23_rev</t>
+  </si>
+  <si>
+    <t>P24_fwd</t>
+  </si>
+  <si>
+    <t>P24_rev</t>
+  </si>
+  <si>
+    <t>P25_fwd</t>
+  </si>
+  <si>
+    <t>P25_rev</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -697,6 +775,12 @@
       <color theme="1"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1045,15 +1129,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F70325E2-930A-4FF1-9E0A-1F1940F58E72}">
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B58"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="2" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="71.140625" customWidth="1"/>
+    <col min="4" max="4" width="110" customWidth="1"/>
     <col min="5" max="5" width="122.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1118,13 +1202,13 @@
         <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>14</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -1133,1198 +1217,1198 @@
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>11</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>187</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E9" t="s">
-        <v>133</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>188</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E10" t="s">
-        <v>134</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>189</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E11" t="s">
-        <v>135</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>190</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E12" t="s">
-        <v>136</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>191</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E13" t="s">
-        <v>137</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>192</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E14" t="s">
-        <v>138</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>193</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E15" t="s">
-        <v>139</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>194</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E16" t="s">
-        <v>140</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>195</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E17" t="s">
-        <v>141</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>196</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E18" t="s">
-        <v>142</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>197</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E19" t="s">
-        <v>143</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>198</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E20" t="s">
-        <v>144</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>199</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
       </c>
       <c r="D21" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E21" t="s">
-        <v>145</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>
       </c>
       <c r="D22" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E22" t="s">
-        <v>146</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>201</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E23" t="s">
-        <v>147</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>202</v>
       </c>
       <c r="C24" t="s">
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E24" t="s">
-        <v>148</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>203</v>
       </c>
       <c r="C25" t="s">
         <v>7</v>
       </c>
       <c r="D25" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E25" t="s">
-        <v>149</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>204</v>
       </c>
       <c r="C26" t="s">
         <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E26" t="s">
-        <v>150</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>205</v>
       </c>
       <c r="C27" t="s">
         <v>7</v>
       </c>
       <c r="D27" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E27" t="s">
-        <v>151</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>206</v>
       </c>
       <c r="C28" t="s">
         <v>7</v>
       </c>
       <c r="D28" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E28" t="s">
-        <v>152</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" t="s">
-        <v>47</v>
+        <v>207</v>
       </c>
       <c r="C29" t="s">
         <v>7</v>
       </c>
       <c r="D29" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E29" t="s">
-        <v>153</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>208</v>
       </c>
       <c r="C30" t="s">
         <v>7</v>
       </c>
       <c r="D30" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E30" t="s">
-        <v>154</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>209</v>
       </c>
       <c r="C31" t="s">
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E31" t="s">
-        <v>155</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" t="s">
-        <v>50</v>
+        <v>210</v>
       </c>
       <c r="C32" t="s">
         <v>7</v>
       </c>
       <c r="D32" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E32" t="s">
-        <v>156</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" t="s">
-        <v>51</v>
+        <v>211</v>
       </c>
       <c r="C33" t="s">
         <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E33" t="s">
-        <v>157</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" t="s">
-        <v>52</v>
+        <v>212</v>
       </c>
       <c r="C34" t="s">
         <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E34" t="s">
-        <v>158</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" t="s">
-        <v>53</v>
+        <v>213</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
       </c>
       <c r="D35" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E35" t="s">
-        <v>159</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" t="s">
-        <v>54</v>
+        <v>214</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E36" t="s">
-        <v>160</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" t="s">
-        <v>55</v>
+        <v>215</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E37" t="s">
-        <v>161</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>216</v>
       </c>
       <c r="C38" t="s">
         <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E38" t="s">
-        <v>162</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>217</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E39" t="s">
-        <v>163</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" t="s">
-        <v>58</v>
+        <v>218</v>
       </c>
       <c r="C40" t="s">
         <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E40" t="s">
-        <v>164</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" t="s">
-        <v>59</v>
+        <v>219</v>
       </c>
       <c r="C41" t="s">
         <v>7</v>
       </c>
       <c r="D41" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E41" t="s">
-        <v>165</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" t="s">
-        <v>60</v>
+        <v>221</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E42" t="s">
-        <v>166</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" t="s">
-        <v>61</v>
+        <v>222</v>
       </c>
       <c r="C43" t="s">
         <v>7</v>
       </c>
       <c r="D43" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E43" t="s">
-        <v>167</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" t="s">
-        <v>62</v>
+        <v>220</v>
       </c>
       <c r="C44" t="s">
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E44" t="s">
-        <v>168</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" t="s">
-        <v>63</v>
+        <v>223</v>
       </c>
       <c r="C45" t="s">
         <v>7</v>
       </c>
       <c r="D45" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E45" t="s">
-        <v>169</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" t="s">
-        <v>64</v>
+        <v>224</v>
       </c>
       <c r="C46" t="s">
         <v>7</v>
       </c>
       <c r="D46" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E46" t="s">
-        <v>170</v>
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" t="s">
-        <v>65</v>
+        <v>225</v>
       </c>
       <c r="C47" t="s">
         <v>7</v>
       </c>
       <c r="D47" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E47" t="s">
-        <v>171</v>
+        <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" t="s">
-        <v>66</v>
+        <v>226</v>
       </c>
       <c r="C48" t="s">
         <v>7</v>
       </c>
       <c r="D48" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E48" t="s">
-        <v>172</v>
+        <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" t="s">
-        <v>67</v>
+        <v>227</v>
       </c>
       <c r="C49" t="s">
         <v>7</v>
       </c>
       <c r="D49" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E49" t="s">
-        <v>173</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" t="s">
-        <v>68</v>
+        <v>228</v>
       </c>
       <c r="C50" t="s">
         <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E50" t="s">
-        <v>174</v>
+        <v>123</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" t="s">
-        <v>69</v>
+        <v>229</v>
       </c>
       <c r="C51" t="s">
         <v>7</v>
       </c>
       <c r="D51" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E51" t="s">
-        <v>175</v>
+        <v>124</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" t="s">
-        <v>70</v>
+        <v>230</v>
       </c>
       <c r="C52" t="s">
         <v>7</v>
       </c>
       <c r="D52" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E52" t="s">
-        <v>176</v>
+        <v>125</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" t="s">
-        <v>71</v>
+        <v>231</v>
       </c>
       <c r="C53" t="s">
         <v>7</v>
       </c>
       <c r="D53" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E53" t="s">
-        <v>177</v>
+        <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" t="s">
-        <v>72</v>
+        <v>232</v>
       </c>
       <c r="C54" t="s">
         <v>7</v>
       </c>
       <c r="D54" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E54" t="s">
-        <v>178</v>
+        <v>127</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" t="s">
-        <v>73</v>
+        <v>233</v>
       </c>
       <c r="C55" t="s">
         <v>7</v>
       </c>
       <c r="D55" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E55" t="s">
-        <v>179</v>
+        <v>128</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" t="s">
-        <v>74</v>
+        <v>234</v>
       </c>
       <c r="C56" t="s">
         <v>7</v>
       </c>
       <c r="D56" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E56" t="s">
-        <v>180</v>
+        <v>129</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" t="s">
-        <v>75</v>
+        <v>235</v>
       </c>
       <c r="C57" t="s">
         <v>7</v>
       </c>
       <c r="D57" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E57" t="s">
-        <v>181</v>
+        <v>130</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" t="s">
-        <v>76</v>
+        <v>236</v>
       </c>
       <c r="C58" t="s">
         <v>7</v>
       </c>
       <c r="D58" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E58" t="s">
-        <v>182</v>
+        <v>131</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="B59" t="s">
-        <v>79</v>
+        <v>28</v>
       </c>
       <c r="C59" t="s">
         <v>7</v>
       </c>
       <c r="D59" t="s">
-        <v>183</v>
+        <v>132</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" t="s">
-        <v>82</v>
+        <v>31</v>
       </c>
       <c r="C60" t="s">
         <v>7</v>
       </c>
       <c r="D60" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>83</v>
+        <v>32</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="C61" t="s">
         <v>7</v>
       </c>
       <c r="D61" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="C62" t="s">
         <v>7</v>
       </c>
       <c r="D62" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>87</v>
+        <v>36</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" t="s">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="C63" t="s">
         <v>7</v>
       </c>
       <c r="D63" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="C64" t="s">
         <v>7</v>
       </c>
       <c r="D64" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>91</v>
+        <v>40</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" t="s">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C65" t="s">
         <v>7</v>
       </c>
       <c r="D65" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>93</v>
+        <v>42</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" t="s">
-        <v>94</v>
+        <v>43</v>
       </c>
       <c r="C66" t="s">
         <v>7</v>
       </c>
       <c r="D66" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>95</v>
+        <v>44</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="C67" t="s">
         <v>7</v>
       </c>
       <c r="D67" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>97</v>
+        <v>46</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" t="s">
-        <v>98</v>
+        <v>47</v>
       </c>
       <c r="C68" t="s">
         <v>7</v>
       </c>
       <c r="D68" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" t="s">
-        <v>100</v>
+        <v>49</v>
       </c>
       <c r="C69" t="s">
         <v>7</v>
       </c>
       <c r="D69" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>101</v>
+        <v>50</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" t="s">
-        <v>100</v>
+        <v>49</v>
       </c>
       <c r="C70" t="s">
         <v>7</v>
       </c>
       <c r="D70" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>102</v>
+        <v>51</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="C71" t="s">
         <v>7</v>
       </c>
       <c r="D71" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" t="s">
-        <v>105</v>
+        <v>54</v>
       </c>
       <c r="C72" t="s">
         <v>7</v>
       </c>
       <c r="D72" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>106</v>
+        <v>55</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" t="s">
-        <v>107</v>
+        <v>56</v>
       </c>
       <c r="C73" t="s">
         <v>7</v>
       </c>
       <c r="D73" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>108</v>
+        <v>57</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" t="s">
-        <v>109</v>
+        <v>58</v>
       </c>
       <c r="C74" t="s">
         <v>7</v>
       </c>
       <c r="D74" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>110</v>
+        <v>59</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" t="s">
-        <v>111</v>
+        <v>60</v>
       </c>
       <c r="C75" t="s">
         <v>7</v>
       </c>
       <c r="D75" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>112</v>
+        <v>61</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" t="s">
-        <v>113</v>
+        <v>62</v>
       </c>
       <c r="C76" t="s">
         <v>7</v>
       </c>
       <c r="D76" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>114</v>
+        <v>63</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" t="s">
-        <v>115</v>
+        <v>64</v>
       </c>
       <c r="C77" t="s">
         <v>7</v>
       </c>
       <c r="D77" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" t="s">
-        <v>117</v>
+        <v>66</v>
       </c>
       <c r="C78" t="s">
         <v>7</v>
       </c>
       <c r="D78" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>118</v>
+        <v>67</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="B79" t="s">
-        <v>119</v>
+        <v>68</v>
       </c>
       <c r="C79" t="s">
         <v>7</v>
       </c>
       <c r="D79" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>120</v>
+        <v>69</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="B80" t="s">
-        <v>121</v>
+        <v>70</v>
       </c>
       <c r="C80" t="s">
         <v>7</v>
       </c>
       <c r="D80" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>122</v>
+        <v>71</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
       <c r="B81" t="s">
-        <v>123</v>
+        <v>72</v>
       </c>
       <c r="C81" t="s">
         <v>7</v>
       </c>
       <c r="D81" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>124</v>
+        <v>73</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="B82" t="s">
-        <v>125</v>
+        <v>74</v>
       </c>
       <c r="C82" t="s">
         <v>7</v>
       </c>
       <c r="D82" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>126</v>
+        <v>75</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
       <c r="B83" t="s">
-        <v>127</v>
+        <v>76</v>
       </c>
       <c r="C83" t="s">
         <v>7</v>
       </c>
       <c r="D83" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>128</v>
+        <v>77</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="B84" t="s">
-        <v>129</v>
+        <v>78</v>
       </c>
       <c r="C84" t="s">
         <v>7</v>
       </c>
       <c r="D84" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>131</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2335,6 +2419,7 @@
     <mergeCell ref="A9:A58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2342,221 +2427,222 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{242A1BDA-9E00-4EC4-9F1C-55DCBBE0F406}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>167</v>
+      </c>
+      <c r="B9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>168</v>
+      </c>
+      <c r="B10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>169</v>
+      </c>
+      <c r="B11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>170</v>
+      </c>
+      <c r="B12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>171</v>
+      </c>
+      <c r="B13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>172</v>
+      </c>
+      <c r="B14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>173</v>
+      </c>
+      <c r="B15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>174</v>
+      </c>
+      <c r="B16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>175</v>
+      </c>
+      <c r="B17" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>176</v>
+      </c>
+      <c r="B18" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>177</v>
+      </c>
+      <c r="B19" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B20" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>179</v>
+      </c>
+      <c r="B21" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>180</v>
+      </c>
+      <c r="B22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>181</v>
+      </c>
+      <c r="B23" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>182</v>
+      </c>
+      <c r="B24" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>183</v>
+      </c>
+      <c r="B25" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>184</v>
       </c>
-      <c r="B1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>75</v>
-      </c>
-      <c r="B2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>52</v>
-      </c>
-      <c r="B6" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>72</v>
-      </c>
-      <c r="B7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>55</v>
-      </c>
-      <c r="B9" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>45</v>
-      </c>
-      <c r="B11" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>64</v>
-      </c>
-      <c r="B12" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>6</v>
-      </c>
-      <c r="B13" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>29</v>
-      </c>
-      <c r="B14" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>24</v>
-      </c>
-      <c r="B15" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>20</v>
-      </c>
-      <c r="B16" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>76</v>
-      </c>
-      <c r="B18" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>11</v>
-      </c>
-      <c r="B19" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>59</v>
-      </c>
-      <c r="B20" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>26</v>
-      </c>
-      <c r="B21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>58</v>
-      </c>
-      <c r="B22" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>30</v>
-      </c>
-      <c r="B23" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>73</v>
-      </c>
-      <c r="B24" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>38</v>
-      </c>
-      <c r="B25" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>78</v>
-      </c>
       <c r="B26" t="s">
-        <v>210</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>